<commit_message>
Add breaks data for kids and fix task names
</commit_message>
<xml_diff>
--- a/children/results_children.xlsx
+++ b/children/results_children.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kv301\Documents\comparative-object-permanence\children\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11975923-A4AC-4255-A029-08E7D465496F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E2C3A7-3645-4098-AA3C-FC87E42783B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
+    <workbookView xWindow="-24120" yWindow="-5655" windowWidth="24240" windowHeight="13020" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,9 +347,6 @@
     <t>OP-STC-Allo-CVChick-Low-Left-Grey-0-OPQ</t>
   </si>
   <si>
-    <t>OP-STC-Allo-PCTB-3CupFC-2G2LRFar-DarkBlue-0-OpLava</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-PCTB-3CupFC-1G2MClose-Grey-0-OPQ</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>OP-STC-Allo-PCTB-4CupGridClose-G2FarLeft-NA-0-NA</t>
   </si>
   <si>
-    <t>OP-STC-Allo-PCTB-3CupFC-2G2MRFar-Brown-0-OPQ</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-CVChick-1Occluder-Right-RND-0-OPQ</t>
   </si>
   <si>
@@ -401,18 +395,9 @@
     <t>OP-STC-Allo-CVChick-1Occluder-Left-Grey-0-OPQ</t>
   </si>
   <si>
-    <t>OP-STC-Allo-PCTB-3CupFC-2G2LMFar-DarkBlue-0-OpLava</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-PCTB-3CupFC-1G2LClose-DarkBlue-0-OpLava</t>
   </si>
   <si>
-    <t>OP-STC-Allo-PCTB-3CupFC-2G2LMClose-DarkGreen-0-OPQ</t>
-  </si>
-  <si>
-    <t>OP-STC-Allo-PCTB-3CupFC-2G2MRClose-DarkBlue-0-OPQ</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-PCTB-12CupGrid-G2FarLeft-G2Far-NA-0-NA</t>
   </si>
   <si>
@@ -543,6 +528,21 @@
   </si>
   <si>
     <t>tutorial_0_ready-G2-sanity_3</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-3CupFC-2Y2MRFar-Brown-0-OPQ</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-3CupFC-2Y2LMClose-DarkGreen-0-OPQ</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-3CupFC-2Y2LMFar-DarkBlue-0-OpLava</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-3CupFC-2Y2MRClose-DarkBlue-0-OPQ</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-3CupFC-2Y2LRFar-DarkBlue-0-OpLava</t>
   </si>
 </sst>
 </file>
@@ -806,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -831,64 +831,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -914,6 +867,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1233,8 +1228,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z16" sqref="Z16"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CK2" sqref="CK2:CK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,595 +1279,592 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:98" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="24"/>
-      <c r="BL1" s="24"/>
-      <c r="BM1" s="24"/>
-      <c r="BN1" s="24"/>
-      <c r="BO1" s="24"/>
-      <c r="BP1" s="24"/>
-      <c r="BQ1" s="24"/>
-      <c r="BR1" s="24"/>
-      <c r="BS1" s="24"/>
-      <c r="BT1" s="24"/>
-      <c r="BU1" s="24"/>
-      <c r="BV1" s="24"/>
-      <c r="BW1" s="24"/>
-      <c r="BX1" s="24"/>
-      <c r="BY1" s="24"/>
-      <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-      <c r="CD1" s="24"/>
-      <c r="CE1" s="24"/>
-      <c r="CF1" s="24"/>
-      <c r="CG1" s="24"/>
-      <c r="CH1" s="24"/>
-      <c r="CI1" s="24"/>
-      <c r="CJ1" s="24"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="X1" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AV1" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="AW1" s="34"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="34"/>
+      <c r="AZ1" s="34"/>
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="34"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="34"/>
+      <c r="BT1" s="34"/>
+      <c r="BU1" s="34"/>
+      <c r="BV1" s="34"/>
+      <c r="BW1" s="34"/>
+      <c r="BX1" s="34"/>
+      <c r="BY1" s="34"/>
+      <c r="BZ1" s="34"/>
+      <c r="CA1" s="34"/>
+      <c r="CB1" s="34"/>
+      <c r="CC1" s="34"/>
+      <c r="CD1" s="34"/>
+      <c r="CE1" s="34"/>
+      <c r="CF1" s="34"/>
+      <c r="CG1" s="34"/>
+      <c r="CH1" s="34"/>
+      <c r="CI1" s="34"/>
+      <c r="CJ1" s="34"/>
     </row>
-    <row r="2" spans="1:98" s="28" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="1:98" s="17" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="39" t="s">
+      <c r="AC2" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD2" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="Y2" s="40" t="s">
+      <c r="AE2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG2" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH2" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI2" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ2" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK2" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL2" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM2" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="AN2" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="Z2" s="40" t="s">
+      <c r="AO2" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="AP2" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="AA2" s="40" t="s">
+      <c r="AQ2" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="AB2" s="40" t="s">
+      <c r="AR2" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="AC2" s="40" t="s">
+      <c r="AS2" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="AD2" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE2" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF2" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG2" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="AH2" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="AI2" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ2" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="AK2" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="AL2" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="AM2" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="AN2" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO2" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP2" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ2" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR2" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="AS2" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="AT2" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="AU2" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="AV2" s="27" t="s">
+      <c r="AT2" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AW2" s="27" t="s">
+      <c r="AW2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="AX2" s="27" t="s">
+      <c r="AX2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AY2" s="27" t="s">
+      <c r="AY2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AZ2" s="27" t="s">
+      <c r="AZ2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="BA2" s="27" t="s">
+      <c r="BA2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="BB2" s="27" t="s">
+      <c r="BB2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="BC2" s="27" t="s">
+      <c r="BC2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="BD2" s="27" t="s">
+      <c r="BD2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="BE2" s="27" t="s">
+      <c r="BE2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="BF2" s="19" t="s">
+      <c r="BF2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="BG2" s="27" t="s">
+      <c r="BG2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="BH2" s="27" t="s">
+      <c r="BH2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="BI2" s="27" t="s">
+      <c r="BI2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="BJ2" s="27" t="s">
+      <c r="BJ2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="BK2" s="27" t="s">
+      <c r="BK2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="BL2" s="27" t="s">
+      <c r="BL2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="BM2" s="27" t="s">
+      <c r="BM2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="BN2" s="27" t="s">
+      <c r="BN2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="BO2" s="27" t="s">
+      <c r="BO2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="BP2" s="27" t="s">
+      <c r="BP2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="BQ2" s="19" t="s">
+      <c r="BQ2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="BR2" s="27" t="s">
+      <c r="BR2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="BS2" s="27" t="s">
+      <c r="BS2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="BT2" s="27" t="s">
+      <c r="BT2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="BU2" s="27" t="s">
+      <c r="BU2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="BV2" s="27" t="s">
+      <c r="BV2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="BW2" s="27" t="s">
+      <c r="BW2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="BX2" s="27" t="s">
+      <c r="BX2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="BY2" s="27" t="s">
+      <c r="BY2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="BZ2" s="27" t="s">
+      <c r="BZ2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="CA2" s="27" t="s">
+      <c r="CA2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="CB2" s="19" t="s">
+      <c r="CB2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="CC2" s="27" t="s">
+      <c r="CC2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="CD2" s="27" t="s">
+      <c r="CD2" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="CE2" s="27" t="s">
+      <c r="CE2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="CF2" s="27" t="s">
+      <c r="CF2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="CG2" s="27" t="s">
+      <c r="CG2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="CH2" s="27" t="s">
+      <c r="CH2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="CI2" s="27" t="s">
+      <c r="CI2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="CJ2" s="27" t="s">
+      <c r="CJ2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="CK2" s="19" t="s">
-        <v>130</v>
+      <c r="CK2" s="30" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:98" s="11" customFormat="1" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="O3" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="Q3" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="R3" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S3" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="T3" s="33" t="s">
+      <c r="T3" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="U3" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="V3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="W3" s="34"/>
-      <c r="X3" s="42" t="s">
+      <c r="W3" s="42"/>
+      <c r="X3" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y3" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="Y3" s="43" t="s">
+      <c r="AD3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="Z3" s="43" t="s">
+      <c r="AE3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="AA3" s="43" t="s">
+      <c r="AF3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AB3" s="43" t="s">
+      <c r="AG3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="AC3" s="43" t="s">
+      <c r="AH3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="AD3" s="43" t="s">
+      <c r="AI3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AE3" s="43" t="s">
+      <c r="AJ3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="AF3" s="43" t="s">
+      <c r="AK3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="AG3" s="43" t="s">
+      <c r="AL3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="AH3" s="43" t="s">
+      <c r="AM3" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="AI3" s="43" t="s">
+      <c r="AN3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="AJ3" s="43" t="s">
+      <c r="AO3" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="AK3" s="43" t="s">
+      <c r="AP3" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="AL3" s="43" t="s">
+      <c r="AQ3" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="AM3" s="43" t="s">
+      <c r="AR3" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="AN3" s="43" t="s">
+      <c r="AS3" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="AO3" s="43" t="s">
+      <c r="AT3" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="AP3" s="43" t="s">
+      <c r="AU3" s="33"/>
+      <c r="AV3" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW3" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX3" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="AY3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ3" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA3" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="BB3" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD3" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="BE3" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="AQ3" s="43" t="s">
+      <c r="BF3" s="31"/>
+      <c r="BG3" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="BH3" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="BI3" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="BJ3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="BK3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="BL3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="BM3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="BN3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="BO3" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="BP3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="BQ3" s="31"/>
+      <c r="BR3" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="BS3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT3" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="BV3" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="BW3" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="AR3" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="AS3" s="43" t="s">
+      <c r="BX3" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="BY3" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="BZ3" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="AT3" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="AU3" s="35"/>
-      <c r="AV3" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW3" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="AX3" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="AY3" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="AZ3" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA3" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="BB3" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="BC3" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="BD3" s="36" t="s">
+      <c r="CA3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="CB3" s="31"/>
+      <c r="CC3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="CD3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="CE3" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="CF3" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="CG3" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="CH3" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="CI3" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="CJ3" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="BE3" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="BF3" s="37"/>
-      <c r="BG3" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="BH3" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="BI3" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="BJ3" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="BK3" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="BL3" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="BM3" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="BN3" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="BO3" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="BP3" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="BQ3" s="37"/>
-      <c r="BR3" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="BS3" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="BT3" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="BU3" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="BV3" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="BW3" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="BX3" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="BY3" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="BZ3" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="CA3" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="CB3" s="37"/>
-      <c r="CC3" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="CD3" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="CE3" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="CF3" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="CG3" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="CH3" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="CI3" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="CJ3" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="CK3" s="37"/>
-      <c r="CL3" s="38"/>
-      <c r="CM3" s="38"/>
-      <c r="CN3" s="38"/>
-      <c r="CO3" s="38"/>
-      <c r="CP3" s="38"/>
-      <c r="CQ3" s="38"/>
-      <c r="CR3" s="38"/>
-      <c r="CS3" s="38"/>
-      <c r="CT3" s="38"/>
+      <c r="CK3" s="31"/>
+      <c r="CL3" s="21"/>
+      <c r="CM3" s="21"/>
+      <c r="CN3" s="21"/>
+      <c r="CO3" s="21"/>
+      <c r="CP3" s="21"/>
+      <c r="CQ3" s="21"/>
+      <c r="CR3" s="21"/>
+      <c r="CS3" s="21"/>
+      <c r="CT3" s="21"/>
     </row>
     <row r="4" spans="1:98" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1980,18 +1972,20 @@
       <c r="AI4" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ4" s="45"/>
-      <c r="AK4" s="45"/>
-      <c r="AL4" s="45"/>
-      <c r="AM4" s="45"/>
-      <c r="AN4" s="45"/>
-      <c r="AO4" s="45"/>
-      <c r="AP4" s="45"/>
-      <c r="AQ4" s="45"/>
-      <c r="AR4" s="45"/>
-      <c r="AS4" s="45"/>
-      <c r="AT4" s="45"/>
-      <c r="AU4" s="2"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="28"/>
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="28"/>
+      <c r="AO4" s="28"/>
+      <c r="AP4" s="28"/>
+      <c r="AQ4" s="28"/>
+      <c r="AR4" s="28"/>
+      <c r="AS4" s="28"/>
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV4" s="5">
         <v>1.618395</v>
       </c>
@@ -2022,7 +2016,9 @@
       <c r="BE4" s="5">
         <v>3.528152</v>
       </c>
-      <c r="BF4" s="12"/>
+      <c r="BF4" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG4" s="3">
         <v>2.6027939999999998</v>
       </c>
@@ -2053,7 +2049,9 @@
       <c r="BP4" s="3">
         <v>-1.0001409999999999</v>
       </c>
-      <c r="BQ4" s="14"/>
+      <c r="BQ4" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR4" s="3">
         <v>-1.1832020000000001</v>
       </c>
@@ -2084,7 +2082,9 @@
       <c r="CA4" s="3">
         <v>2.8251979999999999</v>
       </c>
-      <c r="CB4" s="14"/>
+      <c r="CB4" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC4" s="5">
         <v>1.110787</v>
       </c>
@@ -2106,7 +2106,7 @@
       <c r="CI4" s="5">
         <v>1.8325979999999999</v>
       </c>
-      <c r="CJ4" s="25">
+      <c r="CJ4" s="3">
         <v>2.7553969999999999</v>
       </c>
       <c r="CK4" s="14"/>
@@ -2217,18 +2217,20 @@
       <c r="AI5" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="45"/>
-      <c r="AL5" s="45"/>
-      <c r="AM5" s="45"/>
-      <c r="AN5" s="45"/>
-      <c r="AO5" s="45"/>
-      <c r="AP5" s="45"/>
-      <c r="AQ5" s="45"/>
-      <c r="AR5" s="45"/>
-      <c r="AS5" s="45"/>
-      <c r="AT5" s="45"/>
-      <c r="AU5" s="2"/>
+      <c r="AJ5" s="28"/>
+      <c r="AK5" s="28"/>
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28"/>
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV5" s="5">
         <v>1.812198</v>
       </c>
@@ -2259,7 +2261,9 @@
       <c r="BE5" s="5">
         <v>3.5931540000000002</v>
       </c>
-      <c r="BF5" s="12"/>
+      <c r="BF5" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG5" s="3">
         <v>2.8959990000000002</v>
       </c>
@@ -2290,7 +2294,9 @@
       <c r="BP5" s="3">
         <v>2.8191980000000001</v>
       </c>
-      <c r="BQ5" s="14"/>
+      <c r="BQ5" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR5" s="3">
         <v>2.7937979999999998</v>
       </c>
@@ -2321,7 +2327,9 @@
       <c r="CA5" s="3">
         <v>2.7161960000000001</v>
       </c>
-      <c r="CB5" s="14"/>
+      <c r="CB5" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC5" s="5">
         <v>1.5435950000000001</v>
       </c>
@@ -2451,19 +2459,21 @@
       <c r="AH6" s="2">
         <v>-1.0000119999999999</v>
       </c>
-      <c r="AI6" s="45"/>
-      <c r="AJ6" s="45"/>
-      <c r="AK6" s="45"/>
-      <c r="AL6" s="45"/>
-      <c r="AM6" s="45"/>
-      <c r="AN6" s="45"/>
-      <c r="AO6" s="45"/>
-      <c r="AP6" s="45"/>
-      <c r="AQ6" s="45"/>
-      <c r="AR6" s="45"/>
-      <c r="AS6" s="45"/>
-      <c r="AT6" s="45"/>
-      <c r="AU6" s="2"/>
+      <c r="AI6" s="28"/>
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="28"/>
+      <c r="AL6" s="28"/>
+      <c r="AM6" s="28"/>
+      <c r="AN6" s="28"/>
+      <c r="AO6" s="28"/>
+      <c r="AP6" s="28"/>
+      <c r="AQ6" s="28"/>
+      <c r="AR6" s="28"/>
+      <c r="AS6" s="28"/>
+      <c r="AT6" s="28"/>
+      <c r="AU6" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV6" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -2484,7 +2494,7 @@
       <c r="BC6" s="4"/>
       <c r="BD6" s="4"/>
       <c r="BE6" s="4"/>
-      <c r="BF6" s="12"/>
+      <c r="BF6" s="4"/>
       <c r="BG6" s="4"/>
       <c r="BH6" s="4"/>
       <c r="BI6" s="4"/>
@@ -2495,7 +2505,7 @@
       <c r="BN6" s="4"/>
       <c r="BO6" s="4"/>
       <c r="BP6" s="4"/>
-      <c r="BQ6" s="14"/>
+      <c r="BQ6" s="4"/>
       <c r="BR6" s="4"/>
       <c r="BS6" s="4"/>
       <c r="BT6" s="4"/>
@@ -2506,7 +2516,7 @@
       <c r="BY6" s="4"/>
       <c r="BZ6" s="4"/>
       <c r="CA6" s="4"/>
-      <c r="CB6" s="14"/>
+      <c r="CB6" s="4"/>
       <c r="CC6" s="4"/>
       <c r="CD6" s="4"/>
       <c r="CE6" s="4"/>
@@ -2620,19 +2630,21 @@
       <c r="AH7" s="2">
         <v>1.4443950000000001</v>
       </c>
-      <c r="AI7" s="45"/>
-      <c r="AJ7" s="45"/>
-      <c r="AK7" s="45"/>
-      <c r="AL7" s="45"/>
-      <c r="AM7" s="45"/>
-      <c r="AN7" s="45"/>
-      <c r="AO7" s="45"/>
-      <c r="AP7" s="45"/>
-      <c r="AQ7" s="45"/>
-      <c r="AR7" s="45"/>
-      <c r="AS7" s="45"/>
-      <c r="AT7" s="45"/>
-      <c r="AU7" s="2"/>
+      <c r="AI7" s="28"/>
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="28"/>
+      <c r="AL7" s="28"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="28"/>
+      <c r="AO7" s="28"/>
+      <c r="AP7" s="28"/>
+      <c r="AQ7" s="28"/>
+      <c r="AR7" s="28"/>
+      <c r="AS7" s="28"/>
+      <c r="AT7" s="28"/>
+      <c r="AU7" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV7" s="5">
         <v>1.813598</v>
       </c>
@@ -2663,7 +2675,9 @@
       <c r="BE7" s="5">
         <v>0.76790049999999999</v>
       </c>
-      <c r="BF7" s="12"/>
+      <c r="BF7" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG7" s="3">
         <v>2.8275980000000001</v>
       </c>
@@ -2694,7 +2708,9 @@
       <c r="BP7" s="3">
         <v>2.9159999999999999</v>
       </c>
-      <c r="BQ7" s="14"/>
+      <c r="BQ7" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR7" s="3">
         <v>-1.2330030000000001</v>
       </c>
@@ -2725,7 +2741,9 @@
       <c r="CA7" s="3">
         <v>2.8063980000000002</v>
       </c>
-      <c r="CB7" s="14"/>
+      <c r="CB7" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC7" s="5">
         <v>1.396792</v>
       </c>
@@ -2888,8 +2906,10 @@
       <c r="AS8" s="2">
         <v>-1.0000119999999999</v>
       </c>
-      <c r="AT8" s="45"/>
-      <c r="AU8" s="2"/>
+      <c r="AT8" s="28"/>
+      <c r="AU8" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV8" s="5">
         <v>1.887799</v>
       </c>
@@ -2920,7 +2940,9 @@
       <c r="BE8" s="5">
         <v>3.5823499999999999</v>
       </c>
-      <c r="BF8" s="12"/>
+      <c r="BF8" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG8" s="3">
         <v>-1.171802</v>
       </c>
@@ -2951,7 +2973,9 @@
       <c r="BP8" s="3">
         <v>2.877799</v>
       </c>
-      <c r="BQ8" s="14"/>
+      <c r="BQ8" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR8" s="3">
         <v>2.8011979999999999</v>
       </c>
@@ -2982,7 +3006,9 @@
       <c r="CA8" s="3">
         <v>-1.466807</v>
       </c>
-      <c r="CB8" s="14"/>
+      <c r="CB8" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC8" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -3145,8 +3171,10 @@
       <c r="AS9" s="2">
         <v>-1.0000119999999999</v>
       </c>
-      <c r="AT9" s="45"/>
-      <c r="AU9" s="2"/>
+      <c r="AT9" s="28"/>
+      <c r="AU9" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV9" s="5">
         <v>1.450399</v>
       </c>
@@ -3177,7 +3205,9 @@
       <c r="BE9" s="5">
         <v>2.9826709999999999</v>
       </c>
-      <c r="BF9" s="12"/>
+      <c r="BF9" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG9" s="3">
         <v>2.5493939999999999</v>
       </c>
@@ -3208,7 +3238,9 @@
       <c r="BP9" s="3">
         <v>2.6861959999999998</v>
       </c>
-      <c r="BQ9" s="14"/>
+      <c r="BQ9" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR9" s="3">
         <v>2.7559969999999998</v>
       </c>
@@ -3239,7 +3271,9 @@
       <c r="CA9" s="3">
         <v>2.7523970000000002</v>
       </c>
-      <c r="CB9" s="14"/>
+      <c r="CB9" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC9" s="5">
         <v>1.4039919999999999</v>
       </c>
@@ -3402,8 +3436,10 @@
       <c r="AS10" s="2">
         <v>1.5315970000000001</v>
       </c>
-      <c r="AT10" s="45"/>
-      <c r="AU10" s="2"/>
+      <c r="AT10" s="28"/>
+      <c r="AU10" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV10" s="5">
         <v>1.8607990000000001</v>
       </c>
@@ -3434,7 +3470,9 @@
       <c r="BE10" s="5">
         <v>3.5505580000000001</v>
       </c>
-      <c r="BF10" s="12"/>
+      <c r="BF10" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG10" s="3">
         <v>2.8247979999999999</v>
       </c>
@@ -3465,7 +3503,9 @@
       <c r="BP10" s="3">
         <v>2.7613970000000001</v>
       </c>
-      <c r="BQ10" s="14"/>
+      <c r="BQ10" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR10" s="3">
         <v>2.7815970000000001</v>
       </c>
@@ -3496,7 +3536,9 @@
       <c r="CA10" s="3">
         <v>2.837399</v>
       </c>
-      <c r="CB10" s="14"/>
+      <c r="CB10" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC10" s="5">
         <v>1.4655929999999999</v>
       </c>
@@ -3632,17 +3674,19 @@
       <c r="AJ11" s="2">
         <v>1.998</v>
       </c>
-      <c r="AK11" s="45"/>
-      <c r="AL11" s="45"/>
-      <c r="AM11" s="45"/>
-      <c r="AN11" s="45"/>
-      <c r="AO11" s="45"/>
-      <c r="AP11" s="45"/>
-      <c r="AQ11" s="45"/>
-      <c r="AR11" s="45"/>
-      <c r="AS11" s="45"/>
-      <c r="AT11" s="45"/>
-      <c r="AU11" s="2"/>
+      <c r="AK11" s="28"/>
+      <c r="AL11" s="28"/>
+      <c r="AM11" s="28"/>
+      <c r="AN11" s="28"/>
+      <c r="AO11" s="28"/>
+      <c r="AP11" s="28"/>
+      <c r="AQ11" s="28"/>
+      <c r="AR11" s="28"/>
+      <c r="AS11" s="28"/>
+      <c r="AT11" s="28"/>
+      <c r="AU11" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV11" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -3673,7 +3717,9 @@
       <c r="BE11" s="5">
         <v>3.3613110000000002</v>
       </c>
-      <c r="BF11" s="12"/>
+      <c r="BF11" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG11" s="3">
         <v>2.6257950000000001</v>
       </c>
@@ -3704,7 +3750,9 @@
       <c r="BP11" s="3">
         <v>2.6495950000000001</v>
       </c>
-      <c r="BQ11" s="14"/>
+      <c r="BQ11" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR11" s="3">
         <v>2.7893979999999998</v>
       </c>
@@ -3735,7 +3783,9 @@
       <c r="CA11" s="3">
         <v>2.9161999999999999</v>
       </c>
-      <c r="CB11" s="14"/>
+      <c r="CB11" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC11" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -3871,17 +3921,19 @@
       <c r="AJ12" s="2">
         <v>1.998</v>
       </c>
-      <c r="AK12" s="45"/>
-      <c r="AL12" s="45"/>
-      <c r="AM12" s="45"/>
-      <c r="AN12" s="45"/>
-      <c r="AO12" s="45"/>
-      <c r="AP12" s="45"/>
-      <c r="AQ12" s="45"/>
-      <c r="AR12" s="45"/>
-      <c r="AS12" s="45"/>
-      <c r="AT12" s="45"/>
-      <c r="AU12" s="2"/>
+      <c r="AK12" s="28"/>
+      <c r="AL12" s="28"/>
+      <c r="AM12" s="28"/>
+      <c r="AN12" s="28"/>
+      <c r="AO12" s="28"/>
+      <c r="AP12" s="28"/>
+      <c r="AQ12" s="28"/>
+      <c r="AR12" s="28"/>
+      <c r="AS12" s="28"/>
+      <c r="AT12" s="28"/>
+      <c r="AU12" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV12" s="5">
         <v>1.867799</v>
       </c>
@@ -3912,7 +3964,9 @@
       <c r="BE12" s="5">
         <v>3.6249669999999998</v>
       </c>
-      <c r="BF12" s="12"/>
+      <c r="BF12" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG12" s="3">
         <v>-1.158401</v>
       </c>
@@ -3943,7 +3997,9 @@
       <c r="BP12" s="3">
         <v>2.8991989999999999</v>
       </c>
-      <c r="BQ12" s="14"/>
+      <c r="BQ12" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR12" s="3">
         <v>-1.181802</v>
       </c>
@@ -3974,7 +4030,9 @@
       <c r="CA12" s="3">
         <v>2.9076</v>
       </c>
-      <c r="CB12" s="14"/>
+      <c r="CB12" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC12" s="5">
         <v>1.659197</v>
       </c>
@@ -4107,18 +4165,20 @@
       <c r="AI13" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ13" s="45"/>
-      <c r="AK13" s="45"/>
-      <c r="AL13" s="45"/>
-      <c r="AM13" s="45"/>
-      <c r="AN13" s="45"/>
-      <c r="AO13" s="45"/>
-      <c r="AP13" s="45"/>
-      <c r="AQ13" s="45"/>
-      <c r="AR13" s="45"/>
-      <c r="AS13" s="45"/>
-      <c r="AT13" s="45"/>
-      <c r="AU13" s="2"/>
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
+      <c r="AL13" s="28"/>
+      <c r="AM13" s="28"/>
+      <c r="AN13" s="28"/>
+      <c r="AO13" s="28"/>
+      <c r="AP13" s="28"/>
+      <c r="AQ13" s="28"/>
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="28"/>
+      <c r="AT13" s="28"/>
+      <c r="AU13" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV13" s="5">
         <v>1.9112</v>
       </c>
@@ -4149,7 +4209,9 @@
       <c r="BE13" s="5">
         <v>3.8191830000000002</v>
       </c>
-      <c r="BF13" s="12"/>
+      <c r="BF13" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG13" s="3">
         <v>2.8327979999999999</v>
       </c>
@@ -4180,7 +4242,9 @@
       <c r="BP13" s="3">
         <v>2.9159999999999999</v>
       </c>
-      <c r="BQ13" s="14"/>
+      <c r="BQ13" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR13" s="3">
         <v>2.873999</v>
       </c>
@@ -4211,7 +4275,9 @@
       <c r="CA13" s="3">
         <v>2.853599</v>
       </c>
-      <c r="CB13" s="14"/>
+      <c r="CB13" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC13" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -4350,16 +4416,18 @@
       <c r="AK14" s="2">
         <v>-1</v>
       </c>
-      <c r="AL14" s="45"/>
-      <c r="AM14" s="45"/>
-      <c r="AN14" s="45"/>
-      <c r="AO14" s="45"/>
-      <c r="AP14" s="45"/>
-      <c r="AQ14" s="45"/>
-      <c r="AR14" s="45"/>
-      <c r="AS14" s="45"/>
-      <c r="AT14" s="45"/>
-      <c r="AU14" s="2"/>
+      <c r="AL14" s="28"/>
+      <c r="AM14" s="28"/>
+      <c r="AN14" s="28"/>
+      <c r="AO14" s="28"/>
+      <c r="AP14" s="28"/>
+      <c r="AQ14" s="28"/>
+      <c r="AR14" s="28"/>
+      <c r="AS14" s="28"/>
+      <c r="AT14" s="28"/>
+      <c r="AU14" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV14" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -4390,7 +4458,9 @@
       <c r="BE14" s="5">
         <v>3.4543379999999999</v>
       </c>
-      <c r="BF14" s="12"/>
+      <c r="BF14" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG14" s="3">
         <v>-1.237803</v>
       </c>
@@ -4421,7 +4491,9 @@
       <c r="BP14" s="3">
         <v>2.7815970000000001</v>
       </c>
-      <c r="BQ14" s="14"/>
+      <c r="BQ14" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR14" s="3">
         <v>2.8565990000000001</v>
       </c>
@@ -4452,7 +4524,9 @@
       <c r="CA14" s="3">
         <v>2.8191980000000001</v>
       </c>
-      <c r="CB14" s="14"/>
+      <c r="CB14" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC14" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -4585,18 +4659,20 @@
       <c r="AI15" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ15" s="45"/>
-      <c r="AK15" s="45"/>
-      <c r="AL15" s="45"/>
-      <c r="AM15" s="45"/>
-      <c r="AN15" s="45"/>
-      <c r="AO15" s="45"/>
-      <c r="AP15" s="45"/>
-      <c r="AQ15" s="45"/>
-      <c r="AR15" s="45"/>
-      <c r="AS15" s="45"/>
-      <c r="AT15" s="45"/>
-      <c r="AU15" s="2"/>
+      <c r="AJ15" s="28"/>
+      <c r="AK15" s="28"/>
+      <c r="AL15" s="28"/>
+      <c r="AM15" s="28"/>
+      <c r="AN15" s="28"/>
+      <c r="AO15" s="28"/>
+      <c r="AP15" s="28"/>
+      <c r="AQ15" s="28"/>
+      <c r="AR15" s="28"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV15" s="5">
         <v>1.8729990000000001</v>
       </c>
@@ -4627,7 +4703,9 @@
       <c r="BE15" s="5">
         <v>3.8135819999999998</v>
       </c>
-      <c r="BF15" s="12"/>
+      <c r="BF15" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG15" s="3">
         <v>2.9154</v>
       </c>
@@ -4658,7 +4736,9 @@
       <c r="BP15" s="3">
         <v>2.9011999999999998</v>
       </c>
-      <c r="BQ15" s="14"/>
+      <c r="BQ15" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR15" s="3">
         <v>2.9401999999999999</v>
       </c>
@@ -4689,7 +4769,9 @@
       <c r="CA15" s="3">
         <v>2.9108000000000001</v>
       </c>
-      <c r="CB15" s="14"/>
+      <c r="CB15" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC15" s="5">
         <v>1.8311999999999999</v>
       </c>
@@ -4852,8 +4934,10 @@
       <c r="AS16" s="2">
         <v>1.7092000000000001</v>
       </c>
-      <c r="AT16" s="45"/>
-      <c r="AU16" s="2"/>
+      <c r="AT16" s="28"/>
+      <c r="AU16" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV16" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -4884,7 +4968,9 @@
       <c r="BE16" s="5">
         <v>3.3843480000000001</v>
       </c>
-      <c r="BF16" s="12"/>
+      <c r="BF16" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG16" s="3">
         <v>-1.545401</v>
       </c>
@@ -4915,7 +5001,9 @@
       <c r="BP16" s="3">
         <v>2.8461989999999999</v>
       </c>
-      <c r="BQ16" s="14"/>
+      <c r="BQ16" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR16" s="3">
         <v>-1.204602</v>
       </c>
@@ -4946,7 +5034,9 @@
       <c r="CA16" s="3">
         <v>2.7897980000000002</v>
       </c>
-      <c r="CB16" s="14"/>
+      <c r="CB16" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC16" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -5112,7 +5202,9 @@
       <c r="AT17" s="2">
         <v>1.998</v>
       </c>
-      <c r="AU17" s="14"/>
+      <c r="AU17" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV17" s="5">
         <v>1.8025979999999999</v>
       </c>
@@ -5143,7 +5235,9 @@
       <c r="BE17" s="5">
         <v>3.6975669999999998</v>
       </c>
-      <c r="BF17" s="12"/>
+      <c r="BF17" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG17" s="3">
         <v>2.889799</v>
       </c>
@@ -5174,7 +5268,9 @@
       <c r="BP17" s="3">
         <v>2.8871989999999998</v>
       </c>
-      <c r="BQ17" s="14"/>
+      <c r="BQ17" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR17" s="3">
         <v>2.8757990000000002</v>
       </c>
@@ -5205,7 +5301,9 @@
       <c r="CA17" s="3">
         <v>2.8671989999999998</v>
       </c>
-      <c r="CB17" s="14"/>
+      <c r="CB17" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC17" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -5335,19 +5433,21 @@
       <c r="AH18" s="2">
         <v>1.321993</v>
       </c>
-      <c r="AI18" s="45"/>
-      <c r="AJ18" s="45"/>
-      <c r="AK18" s="45"/>
-      <c r="AL18" s="45"/>
-      <c r="AM18" s="45"/>
-      <c r="AN18" s="45"/>
-      <c r="AO18" s="45"/>
-      <c r="AP18" s="45"/>
-      <c r="AQ18" s="45"/>
-      <c r="AR18" s="45"/>
-      <c r="AS18" s="45"/>
-      <c r="AT18" s="45"/>
-      <c r="AU18" s="2"/>
+      <c r="AI18" s="28"/>
+      <c r="AJ18" s="28"/>
+      <c r="AK18" s="28"/>
+      <c r="AL18" s="28"/>
+      <c r="AM18" s="28"/>
+      <c r="AN18" s="28"/>
+      <c r="AO18" s="28"/>
+      <c r="AP18" s="28"/>
+      <c r="AQ18" s="28"/>
+      <c r="AR18" s="28"/>
+      <c r="AS18" s="28"/>
+      <c r="AT18" s="28"/>
+      <c r="AU18" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV18" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -5378,7 +5478,9 @@
       <c r="BE18" s="5">
         <v>3.3509139999999999</v>
       </c>
-      <c r="BF18" s="12"/>
+      <c r="BF18" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG18" s="3">
         <v>-1.350805</v>
       </c>
@@ -5409,7 +5511,9 @@
       <c r="BP18" s="3">
         <v>2.4829949999999998</v>
       </c>
-      <c r="BQ18" s="14"/>
+      <c r="BQ18" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR18" s="3">
         <v>-1.4794069999999999</v>
       </c>
@@ -5440,7 +5544,9 @@
       <c r="CA18" s="3">
         <v>2.8023980000000002</v>
       </c>
-      <c r="CB18" s="14"/>
+      <c r="CB18" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC18" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -5603,8 +5709,10 @@
       <c r="AS19" s="2">
         <v>1.6427989999999999</v>
       </c>
-      <c r="AT19" s="45"/>
-      <c r="AU19" s="2"/>
+      <c r="AT19" s="28"/>
+      <c r="AU19" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV19" s="5">
         <v>1.9359999999999999</v>
       </c>
@@ -5635,7 +5743,9 @@
       <c r="BE19" s="5">
         <v>3.8217829999999999</v>
       </c>
-      <c r="BF19" s="12"/>
+      <c r="BF19" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG19" s="3">
         <v>-1.162202</v>
       </c>
@@ -5666,7 +5776,9 @@
       <c r="BP19" s="3">
         <v>2.9289999999999998</v>
       </c>
-      <c r="BQ19" s="14"/>
+      <c r="BQ19" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR19" s="3">
         <v>2.8555990000000002</v>
       </c>
@@ -5697,7 +5809,9 @@
       <c r="CA19" s="3">
         <v>-1.119801</v>
       </c>
-      <c r="CB19" s="14"/>
+      <c r="CB19" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC19" s="5">
         <v>1.7567980000000001</v>
       </c>
@@ -5827,19 +5941,21 @@
       <c r="AH20" s="2">
         <v>1.4483950000000001</v>
       </c>
-      <c r="AI20" s="45"/>
-      <c r="AJ20" s="45"/>
-      <c r="AK20" s="45"/>
-      <c r="AL20" s="45"/>
-      <c r="AM20" s="45"/>
-      <c r="AN20" s="45"/>
-      <c r="AO20" s="45"/>
-      <c r="AP20" s="45"/>
-      <c r="AQ20" s="45"/>
-      <c r="AR20" s="45"/>
-      <c r="AS20" s="45"/>
-      <c r="AT20" s="45"/>
-      <c r="AU20" s="2"/>
+      <c r="AI20" s="28"/>
+      <c r="AJ20" s="28"/>
+      <c r="AK20" s="28"/>
+      <c r="AL20" s="28"/>
+      <c r="AM20" s="28"/>
+      <c r="AN20" s="28"/>
+      <c r="AO20" s="28"/>
+      <c r="AP20" s="28"/>
+      <c r="AQ20" s="28"/>
+      <c r="AR20" s="28"/>
+      <c r="AS20" s="28"/>
+      <c r="AT20" s="28"/>
+      <c r="AU20" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV20" s="5">
         <v>1.671996</v>
       </c>
@@ -5870,7 +5986,9 @@
       <c r="BE20" s="5">
         <v>0.90046320000000002</v>
       </c>
-      <c r="BF20" s="12"/>
+      <c r="BF20" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG20" s="3">
         <v>2.8421989999999999</v>
       </c>
@@ -5901,7 +6019,9 @@
       <c r="BP20" s="3">
         <v>-1.128201</v>
       </c>
-      <c r="BQ20" s="14"/>
+      <c r="BQ20" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR20" s="3">
         <v>-1.2632030000000001</v>
       </c>
@@ -5932,7 +6052,9 @@
       <c r="CA20" s="3">
         <v>-1.3162039999999999</v>
       </c>
-      <c r="CB20" s="14"/>
+      <c r="CB20" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC20" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -6068,17 +6190,19 @@
       <c r="AJ21" s="2">
         <v>1.998</v>
       </c>
-      <c r="AK21" s="45"/>
-      <c r="AL21" s="45"/>
-      <c r="AM21" s="45"/>
-      <c r="AN21" s="45"/>
-      <c r="AO21" s="45"/>
-      <c r="AP21" s="45"/>
-      <c r="AQ21" s="45"/>
-      <c r="AR21" s="45"/>
-      <c r="AS21" s="45"/>
-      <c r="AT21" s="45"/>
-      <c r="AU21" s="2"/>
+      <c r="AK21" s="28"/>
+      <c r="AL21" s="28"/>
+      <c r="AM21" s="28"/>
+      <c r="AN21" s="28"/>
+      <c r="AO21" s="28"/>
+      <c r="AP21" s="28"/>
+      <c r="AQ21" s="28"/>
+      <c r="AR21" s="28"/>
+      <c r="AS21" s="28"/>
+      <c r="AT21" s="28"/>
+      <c r="AU21" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV21" s="5">
         <v>1.9141999999999999</v>
       </c>
@@ -6109,7 +6233,9 @@
       <c r="BE21" s="5">
         <v>3.774575</v>
       </c>
-      <c r="BF21" s="12"/>
+      <c r="BF21" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG21" s="3">
         <v>-1.0626</v>
       </c>
@@ -6140,7 +6266,9 @@
       <c r="BP21" s="3">
         <v>2.9411999999999998</v>
       </c>
-      <c r="BQ21" s="14"/>
+      <c r="BQ21" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR21" s="3">
         <v>2.903</v>
       </c>
@@ -6171,7 +6299,9 @@
       <c r="CA21" s="3">
         <v>-1.1086009999999999</v>
       </c>
-      <c r="CB21" s="14"/>
+      <c r="CB21" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC21" s="5">
         <v>1.6495960000000001</v>
       </c>
@@ -6301,19 +6431,21 @@
       <c r="AH22" s="2">
         <v>-1.0000119999999999</v>
       </c>
-      <c r="AI22" s="45"/>
-      <c r="AJ22" s="45"/>
-      <c r="AK22" s="45"/>
-      <c r="AL22" s="45"/>
-      <c r="AM22" s="45"/>
-      <c r="AN22" s="45"/>
-      <c r="AO22" s="45"/>
-      <c r="AP22" s="45"/>
-      <c r="AQ22" s="45"/>
-      <c r="AR22" s="45"/>
-      <c r="AS22" s="45"/>
-      <c r="AT22" s="45"/>
-      <c r="AU22" s="2"/>
+      <c r="AI22" s="28"/>
+      <c r="AJ22" s="28"/>
+      <c r="AK22" s="28"/>
+      <c r="AL22" s="28"/>
+      <c r="AM22" s="28"/>
+      <c r="AN22" s="28"/>
+      <c r="AO22" s="28"/>
+      <c r="AP22" s="28"/>
+      <c r="AQ22" s="28"/>
+      <c r="AR22" s="28"/>
+      <c r="AS22" s="28"/>
+      <c r="AT22" s="28"/>
+      <c r="AU22" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV22" s="4"/>
       <c r="AW22" s="4"/>
       <c r="AX22" s="4"/>
@@ -6324,7 +6456,7 @@
       <c r="BC22" s="4"/>
       <c r="BD22" s="4"/>
       <c r="BE22" s="4"/>
-      <c r="BF22" s="12"/>
+      <c r="BF22" s="4"/>
       <c r="BG22" s="4"/>
       <c r="BH22" s="4"/>
       <c r="BI22" s="4"/>
@@ -6341,7 +6473,9 @@
       <c r="BP22" s="3">
         <v>-1.2054020000000001</v>
       </c>
-      <c r="BQ22" s="14"/>
+      <c r="BQ22" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR22" s="3">
         <v>2.3722089999999998</v>
       </c>
@@ -6372,7 +6506,9 @@
       <c r="CA22" s="3">
         <v>2.9226000000000001</v>
       </c>
-      <c r="CB22" s="14"/>
+      <c r="CB22" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC22" s="5">
         <v>1.596395</v>
       </c>
@@ -6511,16 +6647,18 @@
       <c r="AK23" s="2">
         <v>-1</v>
       </c>
-      <c r="AL23" s="45"/>
-      <c r="AM23" s="45"/>
-      <c r="AN23" s="45"/>
-      <c r="AO23" s="45"/>
-      <c r="AP23" s="45"/>
-      <c r="AQ23" s="45"/>
-      <c r="AR23" s="45"/>
-      <c r="AS23" s="45"/>
-      <c r="AT23" s="45"/>
-      <c r="AU23" s="2"/>
+      <c r="AL23" s="28"/>
+      <c r="AM23" s="28"/>
+      <c r="AN23" s="28"/>
+      <c r="AO23" s="28"/>
+      <c r="AP23" s="28"/>
+      <c r="AQ23" s="28"/>
+      <c r="AR23" s="28"/>
+      <c r="AS23" s="28"/>
+      <c r="AT23" s="28"/>
+      <c r="AU23" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV23" s="5">
         <v>1.839599</v>
       </c>
@@ -6551,7 +6689,9 @@
       <c r="BE23" s="5">
         <v>3.5697619999999999</v>
       </c>
-      <c r="BF23" s="12"/>
+      <c r="BF23" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG23" s="3">
         <v>2.9068000000000001</v>
       </c>
@@ -6582,7 +6722,9 @@
       <c r="BP23" s="3">
         <v>2.9174000000000002</v>
       </c>
-      <c r="BQ23" s="14"/>
+      <c r="BQ23" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR23" s="3">
         <v>2.9142000000000001</v>
       </c>
@@ -6613,7 +6755,9 @@
       <c r="CA23" s="3">
         <v>2.807598</v>
       </c>
-      <c r="CB23" s="14"/>
+      <c r="CB23" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC23" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -6746,18 +6890,20 @@
       <c r="AI24" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ24" s="45"/>
-      <c r="AK24" s="45"/>
-      <c r="AL24" s="45"/>
-      <c r="AM24" s="45"/>
-      <c r="AN24" s="45"/>
-      <c r="AO24" s="45"/>
-      <c r="AP24" s="45"/>
-      <c r="AQ24" s="45"/>
-      <c r="AR24" s="45"/>
-      <c r="AS24" s="45"/>
-      <c r="AT24" s="45"/>
-      <c r="AU24" s="2"/>
+      <c r="AJ24" s="28"/>
+      <c r="AK24" s="28"/>
+      <c r="AL24" s="28"/>
+      <c r="AM24" s="28"/>
+      <c r="AN24" s="28"/>
+      <c r="AO24" s="28"/>
+      <c r="AP24" s="28"/>
+      <c r="AQ24" s="28"/>
+      <c r="AR24" s="28"/>
+      <c r="AS24" s="28"/>
+      <c r="AT24" s="28"/>
+      <c r="AU24" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV24" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -6788,7 +6934,9 @@
       <c r="BE24" s="5">
         <v>3.6525629999999998</v>
       </c>
-      <c r="BF24" s="12"/>
+      <c r="BF24" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG24" s="3">
         <v>2.8557990000000002</v>
       </c>
@@ -6819,7 +6967,9 @@
       <c r="BP24" s="3">
         <v>-1.154202</v>
       </c>
-      <c r="BQ24" s="14"/>
+      <c r="BQ24" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR24" s="3">
         <v>-1.1888019999999999</v>
       </c>
@@ -6850,7 +7000,9 @@
       <c r="CA24" s="3">
         <v>-1.179602</v>
       </c>
-      <c r="CB24" s="14"/>
+      <c r="CB24" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC24" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -6983,18 +7135,20 @@
       <c r="AI25" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ25" s="45"/>
-      <c r="AK25" s="45"/>
-      <c r="AL25" s="45"/>
-      <c r="AM25" s="45"/>
-      <c r="AN25" s="45"/>
-      <c r="AO25" s="45"/>
-      <c r="AP25" s="45"/>
-      <c r="AQ25" s="45"/>
-      <c r="AR25" s="45"/>
-      <c r="AS25" s="45"/>
-      <c r="AT25" s="45"/>
-      <c r="AU25" s="2"/>
+      <c r="AJ25" s="28"/>
+      <c r="AK25" s="28"/>
+      <c r="AL25" s="28"/>
+      <c r="AM25" s="28"/>
+      <c r="AN25" s="28"/>
+      <c r="AO25" s="28"/>
+      <c r="AP25" s="28"/>
+      <c r="AQ25" s="28"/>
+      <c r="AR25" s="28"/>
+      <c r="AS25" s="28"/>
+      <c r="AT25" s="28"/>
+      <c r="AU25" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV25" s="4"/>
       <c r="AW25" s="4"/>
       <c r="AX25" s="4"/>
@@ -7005,7 +7159,7 @@
       <c r="BC25" s="4"/>
       <c r="BD25" s="4"/>
       <c r="BE25" s="4"/>
-      <c r="BF25" s="12"/>
+      <c r="BF25" s="4"/>
       <c r="BG25" s="4"/>
       <c r="BH25" s="4"/>
       <c r="BI25" s="4"/>
@@ -7018,7 +7172,9 @@
       <c r="BP25" s="3">
         <v>-0.30340400000000001</v>
       </c>
-      <c r="BQ25" s="14"/>
+      <c r="BQ25" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR25" s="3">
         <v>-1.107801</v>
       </c>
@@ -7049,7 +7205,9 @@
       <c r="CA25" s="3">
         <v>2.8755989999999998</v>
       </c>
-      <c r="CB25" s="14"/>
+      <c r="CB25" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC25" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -7179,19 +7337,21 @@
       <c r="AH26" s="2">
         <v>1.570797</v>
       </c>
-      <c r="AI26" s="45"/>
-      <c r="AJ26" s="45"/>
-      <c r="AK26" s="45"/>
-      <c r="AL26" s="45"/>
-      <c r="AM26" s="45"/>
-      <c r="AN26" s="45"/>
-      <c r="AO26" s="45"/>
-      <c r="AP26" s="45"/>
-      <c r="AQ26" s="45"/>
-      <c r="AR26" s="45"/>
-      <c r="AS26" s="45"/>
-      <c r="AT26" s="45"/>
-      <c r="AU26" s="2"/>
+      <c r="AI26" s="28"/>
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="28"/>
+      <c r="AL26" s="28"/>
+      <c r="AM26" s="28"/>
+      <c r="AN26" s="28"/>
+      <c r="AO26" s="28"/>
+      <c r="AP26" s="28"/>
+      <c r="AQ26" s="28"/>
+      <c r="AR26" s="28"/>
+      <c r="AS26" s="28"/>
+      <c r="AT26" s="28"/>
+      <c r="AU26" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV26" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -7222,7 +7382,9 @@
       <c r="BE26" s="5">
         <v>3.341504</v>
       </c>
-      <c r="BF26" s="12"/>
+      <c r="BF26" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG26" s="3">
         <v>-1.0696000000000001</v>
       </c>
@@ -7253,7 +7415,9 @@
       <c r="BP26" s="3">
         <v>2.791598</v>
       </c>
-      <c r="BQ26" s="14"/>
+      <c r="BQ26" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR26" s="3">
         <v>-1.0804</v>
       </c>
@@ -7284,7 +7448,9 @@
       <c r="CA26" s="3">
         <v>-1.0802</v>
       </c>
-      <c r="CB26" s="14"/>
+      <c r="CB26" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC26" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -7417,18 +7583,20 @@
       <c r="AI27" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ27" s="45"/>
-      <c r="AK27" s="45"/>
-      <c r="AL27" s="45"/>
-      <c r="AM27" s="45"/>
-      <c r="AN27" s="45"/>
-      <c r="AO27" s="45"/>
-      <c r="AP27" s="45"/>
-      <c r="AQ27" s="45"/>
-      <c r="AR27" s="45"/>
-      <c r="AS27" s="45"/>
-      <c r="AT27" s="45"/>
-      <c r="AU27" s="2"/>
+      <c r="AJ27" s="28"/>
+      <c r="AK27" s="28"/>
+      <c r="AL27" s="28"/>
+      <c r="AM27" s="28"/>
+      <c r="AN27" s="28"/>
+      <c r="AO27" s="28"/>
+      <c r="AP27" s="28"/>
+      <c r="AQ27" s="28"/>
+      <c r="AR27" s="28"/>
+      <c r="AS27" s="28"/>
+      <c r="AT27" s="28"/>
+      <c r="AU27" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV27" s="5">
         <v>1.8925989999999999</v>
       </c>
@@ -7459,7 +7627,9 @@
       <c r="BE27" s="5">
         <v>3.7097660000000001</v>
       </c>
-      <c r="BF27" s="12"/>
+      <c r="BF27" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG27" s="3">
         <v>2.8933990000000001</v>
       </c>
@@ -7490,7 +7660,9 @@
       <c r="BP27" s="3">
         <v>2.786597</v>
       </c>
-      <c r="BQ27" s="14"/>
+      <c r="BQ27" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR27" s="3">
         <v>-1.1274010000000001</v>
       </c>
@@ -7521,7 +7693,9 @@
       <c r="CA27" s="3">
         <v>2.8353980000000001</v>
       </c>
-      <c r="CB27" s="14"/>
+      <c r="CB27" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC27" s="5">
         <v>1.7283980000000001</v>
       </c>
@@ -7654,18 +7828,20 @@
       <c r="AI28" s="2">
         <v>1.998</v>
       </c>
-      <c r="AJ28" s="45"/>
-      <c r="AK28" s="45"/>
-      <c r="AL28" s="45"/>
-      <c r="AM28" s="45"/>
-      <c r="AN28" s="45"/>
-      <c r="AO28" s="45"/>
-      <c r="AP28" s="45"/>
-      <c r="AQ28" s="45"/>
-      <c r="AR28" s="45"/>
-      <c r="AS28" s="45"/>
-      <c r="AT28" s="45"/>
-      <c r="AU28" s="2"/>
+      <c r="AJ28" s="28"/>
+      <c r="AK28" s="28"/>
+      <c r="AL28" s="28"/>
+      <c r="AM28" s="28"/>
+      <c r="AN28" s="28"/>
+      <c r="AO28" s="28"/>
+      <c r="AP28" s="28"/>
+      <c r="AQ28" s="28"/>
+      <c r="AR28" s="28"/>
+      <c r="AS28" s="28"/>
+      <c r="AT28" s="28"/>
+      <c r="AU28" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV28" s="5">
         <v>-1.0001409999999999</v>
       </c>
@@ -7696,7 +7872,9 @@
       <c r="BE28" s="5">
         <v>3.341504</v>
       </c>
-      <c r="BF28" s="12"/>
+      <c r="BF28" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG28" s="3">
         <v>2.9508000000000001</v>
       </c>
@@ -7727,7 +7905,9 @@
       <c r="BP28" s="3">
         <v>2.9367999999999999</v>
       </c>
-      <c r="BQ28" s="14"/>
+      <c r="BQ28" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR28" s="3">
         <v>2.886199</v>
       </c>
@@ -7758,7 +7938,9 @@
       <c r="CA28" s="3">
         <v>-1.128001</v>
       </c>
-      <c r="CB28" s="14"/>
+      <c r="CB28" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC28" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -7894,17 +8076,19 @@
       <c r="AJ29" s="2">
         <v>1.998</v>
       </c>
-      <c r="AK29" s="45"/>
-      <c r="AL29" s="45"/>
-      <c r="AM29" s="45"/>
-      <c r="AN29" s="45"/>
-      <c r="AO29" s="45"/>
-      <c r="AP29" s="45"/>
-      <c r="AQ29" s="45"/>
-      <c r="AR29" s="45"/>
-      <c r="AS29" s="45"/>
-      <c r="AT29" s="45"/>
-      <c r="AU29" s="2"/>
+      <c r="AK29" s="28"/>
+      <c r="AL29" s="28"/>
+      <c r="AM29" s="28"/>
+      <c r="AN29" s="28"/>
+      <c r="AO29" s="28"/>
+      <c r="AP29" s="28"/>
+      <c r="AQ29" s="28"/>
+      <c r="AR29" s="28"/>
+      <c r="AS29" s="28"/>
+      <c r="AT29" s="28"/>
+      <c r="AU29" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV29" s="5">
         <v>1.857399</v>
       </c>
@@ -7935,7 +8119,9 @@
       <c r="BE29" s="5">
         <v>0.89126590000000006</v>
       </c>
-      <c r="BF29" s="12"/>
+      <c r="BF29" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG29" s="3">
         <v>-1.1498010000000001</v>
       </c>
@@ -7966,7 +8152,9 @@
       <c r="BP29" s="3">
         <v>2.8803990000000002</v>
       </c>
-      <c r="BQ29" s="14"/>
+      <c r="BQ29" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR29" s="3">
         <v>2.8945989999999999</v>
       </c>
@@ -7997,7 +8185,9 @@
       <c r="CA29" s="3">
         <v>-1.180002</v>
       </c>
-      <c r="CB29" s="14"/>
+      <c r="CB29" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC29" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -8133,17 +8323,19 @@
       <c r="AJ30" s="2">
         <v>1.998</v>
       </c>
-      <c r="AK30" s="45"/>
-      <c r="AL30" s="45"/>
-      <c r="AM30" s="45"/>
-      <c r="AN30" s="45"/>
-      <c r="AO30" s="45"/>
-      <c r="AP30" s="45"/>
-      <c r="AQ30" s="45"/>
-      <c r="AR30" s="45"/>
-      <c r="AS30" s="45"/>
-      <c r="AT30" s="45"/>
-      <c r="AU30" s="2"/>
+      <c r="AK30" s="28"/>
+      <c r="AL30" s="28"/>
+      <c r="AM30" s="28"/>
+      <c r="AN30" s="28"/>
+      <c r="AO30" s="28"/>
+      <c r="AP30" s="28"/>
+      <c r="AQ30" s="28"/>
+      <c r="AR30" s="28"/>
+      <c r="AS30" s="28"/>
+      <c r="AT30" s="28"/>
+      <c r="AU30" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV30" s="5">
         <v>1.857399</v>
       </c>
@@ -8174,7 +8366,9 @@
       <c r="BE30" s="5">
         <v>3.4717319999999998</v>
       </c>
-      <c r="BF30" s="12"/>
+      <c r="BF30" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG30" s="3">
         <v>2.7861980000000002</v>
       </c>
@@ -8205,7 +8399,9 @@
       <c r="BP30" s="3">
         <v>2.8245979999999999</v>
       </c>
-      <c r="BQ30" s="14"/>
+      <c r="BQ30" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR30" s="3">
         <v>2.901599</v>
       </c>
@@ -8236,7 +8432,9 @@
       <c r="CA30" s="3">
         <v>2.787398</v>
       </c>
-      <c r="CB30" s="14"/>
+      <c r="CB30" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC30" s="5">
         <v>1.6271960000000001</v>
       </c>
@@ -8372,17 +8570,19 @@
       <c r="AJ31" s="2">
         <v>1.998</v>
       </c>
-      <c r="AK31" s="45"/>
-      <c r="AL31" s="45"/>
-      <c r="AM31" s="45"/>
-      <c r="AN31" s="45"/>
-      <c r="AO31" s="45"/>
-      <c r="AP31" s="45"/>
-      <c r="AQ31" s="45"/>
-      <c r="AR31" s="45"/>
-      <c r="AS31" s="45"/>
-      <c r="AT31" s="45"/>
-      <c r="AU31" s="2"/>
+      <c r="AK31" s="28"/>
+      <c r="AL31" s="28"/>
+      <c r="AM31" s="28"/>
+      <c r="AN31" s="28"/>
+      <c r="AO31" s="28"/>
+      <c r="AP31" s="28"/>
+      <c r="AQ31" s="28"/>
+      <c r="AR31" s="28"/>
+      <c r="AS31" s="28"/>
+      <c r="AT31" s="28"/>
+      <c r="AU31" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV31" s="5">
         <v>1.8951990000000001</v>
       </c>
@@ -8413,7 +8613,9 @@
       <c r="BE31" s="5">
         <v>3.5445389999999999</v>
       </c>
-      <c r="BF31" s="12"/>
+      <c r="BF31" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG31" s="3">
         <v>2.8223980000000002</v>
       </c>
@@ -8444,7 +8646,9 @@
       <c r="BP31" s="3">
         <v>2.8731990000000001</v>
       </c>
-      <c r="BQ31" s="14"/>
+      <c r="BQ31" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR31" s="3">
         <v>2.791798</v>
       </c>
@@ -8475,7 +8679,9 @@
       <c r="CA31" s="3">
         <v>2.8833989999999998</v>
       </c>
-      <c r="CB31" s="14"/>
+      <c r="CB31" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC31" s="5">
         <v>1.6455960000000001</v>
       </c>
@@ -8605,19 +8811,21 @@
       <c r="AH32" s="2">
         <v>-1.0000119999999999</v>
       </c>
-      <c r="AI32" s="45"/>
-      <c r="AJ32" s="45"/>
-      <c r="AK32" s="45"/>
-      <c r="AL32" s="45"/>
-      <c r="AM32" s="45"/>
-      <c r="AN32" s="45"/>
-      <c r="AO32" s="45"/>
-      <c r="AP32" s="45"/>
-      <c r="AQ32" s="45"/>
-      <c r="AR32" s="45"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="45"/>
-      <c r="AU32" s="2"/>
+      <c r="AI32" s="28"/>
+      <c r="AJ32" s="28"/>
+      <c r="AK32" s="28"/>
+      <c r="AL32" s="28"/>
+      <c r="AM32" s="28"/>
+      <c r="AN32" s="28"/>
+      <c r="AO32" s="28"/>
+      <c r="AP32" s="28"/>
+      <c r="AQ32" s="28"/>
+      <c r="AR32" s="28"/>
+      <c r="AS32" s="28"/>
+      <c r="AT32" s="28"/>
+      <c r="AU32" s="2">
+        <v>1.998</v>
+      </c>
       <c r="AV32" s="5">
         <v>1.881799</v>
       </c>
@@ -8648,7 +8856,9 @@
       <c r="BE32" s="5">
         <v>2.981058</v>
       </c>
-      <c r="BF32" s="12"/>
+      <c r="BF32" s="12">
+        <v>1.998</v>
+      </c>
       <c r="BG32" s="3">
         <v>2.8329979999999999</v>
       </c>
@@ -8679,7 +8889,9 @@
       <c r="BP32" s="3">
         <v>2.8553989999999998</v>
       </c>
-      <c r="BQ32" s="14"/>
+      <c r="BQ32" s="14">
+        <v>1.998</v>
+      </c>
       <c r="BR32" s="3">
         <v>-1.1532009999999999</v>
       </c>
@@ -8710,7 +8922,9 @@
       <c r="CA32" s="3">
         <v>2.749997</v>
       </c>
-      <c r="CB32" s="14"/>
+      <c r="CB32" s="14">
+        <v>1.998</v>
+      </c>
       <c r="CC32" s="5">
         <v>-1.0000150000000001</v>
       </c>
@@ -8846,17 +9060,19 @@
       <c r="AJ33" s="8">
         <v>1.998</v>
       </c>
-      <c r="AK33" s="45"/>
-      <c r="AL33" s="45"/>
-      <c r="AM33" s="45"/>
-      <c r="AN33" s="45"/>
-      <c r="AO33" s="45"/>
-      <c r="AP33" s="45"/>
-      <c r="AQ33" s="45"/>
-      <c r="AR33" s="45"/>
-      <c r="AS33" s="45"/>
-      <c r="AT33" s="45"/>
-      <c r="AU33" s="8"/>
+      <c r="AK33" s="28"/>
+      <c r="AL33" s="28"/>
+      <c r="AM33" s="28"/>
+      <c r="AN33" s="28"/>
+      <c r="AO33" s="28"/>
+      <c r="AP33" s="28"/>
+      <c r="AQ33" s="28"/>
+      <c r="AR33" s="28"/>
+      <c r="AS33" s="28"/>
+      <c r="AT33" s="28"/>
+      <c r="AU33" s="8">
+        <v>1.998</v>
+      </c>
       <c r="AV33" s="9">
         <v>1.656595</v>
       </c>
@@ -8887,7 +9103,9 @@
       <c r="BE33" s="9">
         <v>3.2735539999999999</v>
       </c>
-      <c r="BF33" s="13"/>
+      <c r="BF33" s="13">
+        <v>1.998</v>
+      </c>
       <c r="BG33" s="10">
         <v>2.823798</v>
       </c>
@@ -8918,7 +9136,9 @@
       <c r="BP33" s="10">
         <v>2.7345969999999999</v>
       </c>
-      <c r="BQ33" s="15"/>
+      <c r="BQ33" s="15">
+        <v>1.998</v>
+      </c>
       <c r="BR33" s="10">
         <v>-1.3928050000000001</v>
       </c>
@@ -8949,7 +9169,9 @@
       <c r="CA33" s="10">
         <v>2.742597</v>
       </c>
-      <c r="CB33" s="15"/>
+      <c r="CB33" s="15">
+        <v>1.998</v>
+      </c>
       <c r="CC33" s="9">
         <v>1.409592</v>
       </c>
@@ -8978,6 +9200,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="C1:V1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="X1:AT1"/>
     <mergeCell ref="CK2:CK3"/>
     <mergeCell ref="AU2:AU3"/>
@@ -8985,16 +9217,6 @@
     <mergeCell ref="BQ2:BQ3"/>
     <mergeCell ref="BF2:BF3"/>
     <mergeCell ref="AV1:CJ1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="O2:V2"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="C1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9002,25 +9224,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E74F6B21681AB408F9BC07DC9A0E55C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4c5f0e15b723777ad6492fe9c8c4393">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="03af05c1-6d5e-40c6-b524-3923c3d31a7d" xmlns:ns3="92fb2da0-1efd-490d-9574-64ca626f7778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffba0b7775c6a986b1b6d9a6ba35c06b" ns2:_="" ns3:_="">
     <xsd:import namespace="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
@@ -9225,25 +9428,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF44038-910F-4BF1-8B0A-E9EFAB10C83E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9260,4 +9464,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix metadata names and some minor metadata details
</commit_message>
<xml_diff>
--- a/children/results_children.xlsx
+++ b/children/results_children.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kv301\Documents\comparative-object-permanence\children\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E2C3A7-3645-4098-AA3C-FC87E42783B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB1A54-9F7A-4499-A784-FD1DE48FC150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-5655" windowWidth="24240" windowHeight="13020" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,15 +467,6 @@
     <t>tutorial_1_turning-G2-rightfar_1</t>
   </si>
   <si>
-    <t>tutorial_2_forcedchoice-lavaleft-G2right_1</t>
-  </si>
-  <si>
-    <t>tutorial_3_3choicecylinder-G2-left_1</t>
-  </si>
-  <si>
-    <t>tutorial_4_3choicecylinder-G2-right_1</t>
-  </si>
-  <si>
     <t>tutorial_5_multi-2Y2-left_1</t>
   </si>
   <si>
@@ -543,6 +534,15 @@
   </si>
   <si>
     <t>OP-STC-Allo-PCTB-3CupFC-2Y2LRFar-DarkBlue-0-OpLava</t>
+  </si>
+  <si>
+    <t>tutorial_2_forcedchoice-lavaleft-G2-right_1</t>
+  </si>
+  <si>
+    <t>tutorial_3_3choicecylinder-G1.5-left_1</t>
+  </si>
+  <si>
+    <t>tutorial_4_3choicecylinder-G1.5-right_1</t>
   </si>
 </sst>
 </file>
@@ -868,19 +868,16 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -898,16 +895,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1228,8 +1228,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK2" sqref="CK2:CK3"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,137 +1280,137 @@
   <sheetData>
     <row r="1" spans="1:98" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
-      <c r="C1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="X1" s="29" t="s">
+      <c r="C1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="X1" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AV1" s="34" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AV1" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34"/>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34"/>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="34"/>
-      <c r="BH1" s="34"/>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="34"/>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34"/>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="34"/>
-      <c r="BO1" s="34"/>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="34"/>
-      <c r="BT1" s="34"/>
-      <c r="BU1" s="34"/>
-      <c r="BV1" s="34"/>
-      <c r="BW1" s="34"/>
-      <c r="BX1" s="34"/>
-      <c r="BY1" s="34"/>
-      <c r="BZ1" s="34"/>
-      <c r="CA1" s="34"/>
-      <c r="CB1" s="34"/>
-      <c r="CC1" s="34"/>
-      <c r="CD1" s="34"/>
-      <c r="CE1" s="34"/>
-      <c r="CF1" s="34"/>
-      <c r="CG1" s="34"/>
-      <c r="CH1" s="34"/>
-      <c r="CI1" s="34"/>
-      <c r="CJ1" s="34"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="33"/>
+      <c r="BD1" s="33"/>
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="33"/>
+      <c r="BG1" s="33"/>
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="33"/>
+      <c r="BJ1" s="33"/>
+      <c r="BK1" s="33"/>
+      <c r="BL1" s="33"/>
+      <c r="BM1" s="33"/>
+      <c r="BN1" s="33"/>
+      <c r="BO1" s="33"/>
+      <c r="BP1" s="33"/>
+      <c r="BQ1" s="33"/>
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="33"/>
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="33"/>
+      <c r="BW1" s="33"/>
+      <c r="BX1" s="33"/>
+      <c r="BY1" s="33"/>
+      <c r="BZ1" s="33"/>
+      <c r="CA1" s="33"/>
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="33"/>
+      <c r="CD1" s="33"/>
+      <c r="CE1" s="33"/>
+      <c r="CF1" s="33"/>
+      <c r="CG1" s="33"/>
+      <c r="CH1" s="33"/>
+      <c r="CI1" s="33"/>
+      <c r="CJ1" s="33"/>
     </row>
     <row r="2" spans="1:98" s="17" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="41" t="s">
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="31" t="s">
         <v>8</v>
       </c>
       <c r="X2" s="22" t="s">
@@ -1482,7 +1482,7 @@
       <c r="AT2" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="AU2" s="32" t="s">
+      <c r="AU2" s="41" t="s">
         <v>124</v>
       </c>
       <c r="AV2" s="16" t="s">
@@ -1515,7 +1515,7 @@
       <c r="BE2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="BF2" s="30" t="s">
+      <c r="BF2" s="39" t="s">
         <v>19</v>
       </c>
       <c r="BG2" s="16" t="s">
@@ -1548,7 +1548,7 @@
       <c r="BP2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="BQ2" s="30" t="s">
+      <c r="BQ2" s="39" t="s">
         <v>30</v>
       </c>
       <c r="BR2" s="16" t="s">
@@ -1581,7 +1581,7 @@
       <c r="CA2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="CB2" s="30" t="s">
+      <c r="CB2" s="39" t="s">
         <v>41</v>
       </c>
       <c r="CC2" s="16" t="s">
@@ -1608,17 +1608,17 @@
       <c r="CJ2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="CK2" s="30" t="s">
+      <c r="CK2" s="39" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:98" s="11" customFormat="1" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="19" t="s">
         <v>84</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="V3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="W3" s="42"/>
+      <c r="W3" s="32"/>
       <c r="X3" s="25" t="s">
         <v>141</v>
       </c>
@@ -1675,69 +1675,69 @@
         <v>142</v>
       </c>
       <c r="Z3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC3" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AD3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="AB3" s="26" t="s">
+      <c r="AE3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AC3" s="26" t="s">
+      <c r="AF3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="AD3" s="26" t="s">
+      <c r="AG3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="AE3" s="26" t="s">
+      <c r="AH3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="AF3" s="26" t="s">
+      <c r="AI3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AG3" s="26" t="s">
+      <c r="AJ3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="AH3" s="26" t="s">
+      <c r="AK3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="AI3" s="26" t="s">
+      <c r="AL3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AJ3" s="26" t="s">
+      <c r="AM3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="AK3" s="26" t="s">
+      <c r="AN3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="AL3" s="26" t="s">
+      <c r="AO3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="AM3" s="26" t="s">
+      <c r="AP3" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="AN3" s="26" t="s">
+      <c r="AQ3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="AO3" s="26" t="s">
+      <c r="AR3" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="AP3" s="26" t="s">
+      <c r="AS3" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="AQ3" s="26" t="s">
+      <c r="AT3" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="AR3" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="AS3" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="AT3" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="AU3" s="33"/>
+      <c r="AU3" s="42"/>
       <c r="AV3" s="20" t="s">
         <v>101</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="AX3" s="20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AY3" s="20" t="s">
         <v>103</v>
@@ -1766,9 +1766,9 @@
         <v>108</v>
       </c>
       <c r="BE3" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="BF3" s="31"/>
+        <v>161</v>
+      </c>
+      <c r="BF3" s="40"/>
       <c r="BG3" s="20" t="s">
         <v>109</v>
       </c>
@@ -1799,7 +1799,7 @@
       <c r="BP3" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="BQ3" s="31"/>
+      <c r="BQ3" s="40"/>
       <c r="BR3" s="20" t="s">
         <v>118</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>116</v>
       </c>
       <c r="BT3" s="20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="BU3" s="20" t="s">
         <v>119</v>
@@ -1816,7 +1816,7 @@
         <v>102</v>
       </c>
       <c r="BW3" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="BX3" s="20" t="s">
         <v>104</v>
@@ -1825,12 +1825,12 @@
         <v>105</v>
       </c>
       <c r="BZ3" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="CA3" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="CB3" s="31"/>
+      <c r="CB3" s="40"/>
       <c r="CC3" s="20" t="s">
         <v>120</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="CJ3" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="CK3" s="31"/>
+      <c r="CK3" s="40"/>
       <c r="CL3" s="21"/>
       <c r="CM3" s="21"/>
       <c r="CN3" s="21"/>
@@ -9200,16 +9200,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="O2:V2"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="C1:V1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="X1:AT1"/>
     <mergeCell ref="CK2:CK3"/>
     <mergeCell ref="AU2:AU3"/>
@@ -9217,6 +9207,16 @@
     <mergeCell ref="BQ2:BQ3"/>
     <mergeCell ref="BF2:BF3"/>
     <mergeCell ref="AV1:CJ1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="C1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9224,6 +9224,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E74F6B21681AB408F9BC07DC9A0E55C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4c5f0e15b723777ad6492fe9c8c4393">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="03af05c1-6d5e-40c6-b524-3923c3d31a7d" xmlns:ns3="92fb2da0-1efd-490d-9574-64ca626f7778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffba0b7775c6a986b1b6d9a6ba35c06b" ns2:_="" ns3:_="">
     <xsd:import namespace="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
@@ -9428,26 +9447,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF44038-910F-4BF1-8B0A-E9EFAB10C83E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9464,22 +9482,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix minor error with child tutorial naming convention
</commit_message>
<xml_diff>
--- a/children/results_children.xlsx
+++ b/children/results_children.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kv301\Documents\comparative-object-permanence\children\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB1A54-9F7A-4499-A784-FD1DE48FC150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43289421-4A53-427C-A159-4357B87F5AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
   </bookViews>
@@ -491,15 +491,6 @@
     <t>tutorial_1_turning-G2-rightfar_2</t>
   </si>
   <si>
-    <t>tutorial_2_forcedchoice-lavaleft-G2right_2</t>
-  </si>
-  <si>
-    <t>tutorial_3_3choicecylinder-G2-left_2</t>
-  </si>
-  <si>
-    <t>tutorial_4_3choicecylinder-G2-right_2</t>
-  </si>
-  <si>
     <t>tutorial_5_multi-2Y2-left_2</t>
   </si>
   <si>
@@ -543,6 +534,15 @@
   </si>
   <si>
     <t>tutorial_4_3choicecylinder-G1.5-right_1</t>
+  </si>
+  <si>
+    <t>tutorial_2_forcedchoice-lavaleft-G2-right_2</t>
+  </si>
+  <si>
+    <t>tutorial_3_3choicecylinder-G1.5-left_2</t>
+  </si>
+  <si>
+    <t>tutorial_4_3choicecylinder-G1.5-right_2</t>
   </si>
 </sst>
 </file>
@@ -1228,8 +1228,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB4" sqref="AB4"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1675,13 +1675,13 @@
         <v>142</v>
       </c>
       <c r="Z3" s="26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AA3" s="26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AB3" s="26" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AC3" s="26" t="s">
         <v>143</v>
@@ -1708,34 +1708,34 @@
         <v>150</v>
       </c>
       <c r="AK3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL3" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM3" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="AN3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="AL3" s="26" t="s">
+      <c r="AO3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AM3" s="26" t="s">
+      <c r="AP3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="AN3" s="26" t="s">
+      <c r="AQ3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="AO3" s="26" t="s">
+      <c r="AR3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="AP3" s="26" t="s">
+      <c r="AS3" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="AQ3" s="26" t="s">
+      <c r="AT3" s="27" t="s">
         <v>157</v>
-      </c>
-      <c r="AR3" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="AS3" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="AT3" s="27" t="s">
-        <v>160</v>
       </c>
       <c r="AU3" s="42"/>
       <c r="AV3" s="20" t="s">
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="AX3" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AY3" s="20" t="s">
         <v>103</v>
@@ -1766,7 +1766,7 @@
         <v>108</v>
       </c>
       <c r="BE3" s="20" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="BF3" s="40"/>
       <c r="BG3" s="20" t="s">
@@ -1807,7 +1807,7 @@
         <v>116</v>
       </c>
       <c r="BT3" s="20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="BU3" s="20" t="s">
         <v>119</v>
@@ -1816,7 +1816,7 @@
         <v>102</v>
       </c>
       <c r="BW3" s="20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="BX3" s="20" t="s">
         <v>104</v>
@@ -1825,7 +1825,7 @@
         <v>105</v>
       </c>
       <c r="BZ3" s="20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="CA3" s="20" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Fix error with tutorial 7
</commit_message>
<xml_diff>
--- a/children/results_children.xlsx
+++ b/children/results_children.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kv301\Documents\comparative-object-permanence\children\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43289421-4A53-427C-A159-4357B87F5AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC4FB7F-28FA-41D4-A4E1-A9E2E880B299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
   </bookViews>
@@ -473,9 +473,6 @@
     <t>tutorial_6_OP-RP-Allo-CVChick-G2.52Occluder-Left-Brown-0-OPQ_variant_1</t>
   </si>
   <si>
-    <t>tutorial_7_OP-RP-Allo-CVChick-G2.52Occluder-Left-Brown-0-OPQ_1</t>
-  </si>
-  <si>
     <t>tutorial_8_OP-RP-Allo-PCTB-3CupFCTrans-1G2LClose-NA-0-OpLava_1</t>
   </si>
   <si>
@@ -497,9 +494,6 @@
     <t>tutorial_6_OP-RP-Allo-CVChick-G2.52Occluder-Left-Brown-0-OPQ_variant_2</t>
   </si>
   <si>
-    <t>tutorial_7_OP-RP-Allo-CVChick-G2.52Occluder-Left-Brown-0-OPQ_2</t>
-  </si>
-  <si>
     <t>tutorial_8_OP-RP-Allo-PCTB-3CupFCTrans-1G2LClose-NA-0-OpLava_2</t>
   </si>
   <si>
@@ -543,6 +537,12 @@
   </si>
   <si>
     <t>tutorial_4_3choicecylinder-G1.5-right_2</t>
+  </si>
+  <si>
+    <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_1</t>
+  </si>
+  <si>
+    <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_2</t>
   </si>
 </sst>
 </file>
@@ -1228,8 +1228,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y3" sqref="Y3"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AQ4" sqref="AQ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1675,13 +1675,13 @@
         <v>142</v>
       </c>
       <c r="Z3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB3" s="26" t="s">
         <v>163</v>
-      </c>
-      <c r="AA3" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB3" s="26" t="s">
-        <v>165</v>
       </c>
       <c r="AC3" s="26" t="s">
         <v>143</v>
@@ -1690,52 +1690,52 @@
         <v>144</v>
       </c>
       <c r="AE3" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AF3" s="26" t="s">
+      <c r="AG3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="AG3" s="26" t="s">
+      <c r="AH3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="AH3" s="26" t="s">
+      <c r="AI3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="AI3" s="26" t="s">
+      <c r="AJ3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AJ3" s="26" t="s">
+      <c r="AK3" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL3" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="AM3" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="AN3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="AK3" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="AL3" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="AM3" s="26" t="s">
+      <c r="AO3" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP3" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="AN3" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="AO3" s="26" t="s">
+      <c r="AQ3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AP3" s="26" t="s">
+      <c r="AR3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="AQ3" s="26" t="s">
+      <c r="AS3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="AR3" s="26" t="s">
+      <c r="AT3" s="27" t="s">
         <v>155</v>
-      </c>
-      <c r="AS3" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AT3" s="27" t="s">
-        <v>157</v>
       </c>
       <c r="AU3" s="42"/>
       <c r="AV3" s="20" t="s">
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="AX3" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AY3" s="20" t="s">
         <v>103</v>
@@ -1766,7 +1766,7 @@
         <v>108</v>
       </c>
       <c r="BE3" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="BF3" s="40"/>
       <c r="BG3" s="20" t="s">
@@ -1807,7 +1807,7 @@
         <v>116</v>
       </c>
       <c r="BT3" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="BU3" s="20" t="s">
         <v>119</v>
@@ -1816,7 +1816,7 @@
         <v>102</v>
       </c>
       <c r="BW3" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="BX3" s="20" t="s">
         <v>104</v>
@@ -1825,7 +1825,7 @@
         <v>105</v>
       </c>
       <c r="BZ3" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="CA3" s="20" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
Update error with 12cup grid names in children data
</commit_message>
<xml_diff>
--- a/children/results_children.xlsx
+++ b/children/results_children.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kv301\Documents\comparative-object-permanence\children\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC4FB7F-28FA-41D4-A4E1-A9E2E880B299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC728A0-371B-41F3-BA3A-67112864A102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
   </bookViews>
@@ -359,9 +359,6 @@
     <t>OP-STC-Allo-PCTB-12CupGrid-G2CloseLeftClose-NA-0-NA</t>
   </si>
   <si>
-    <t>OP-STC-Allo-PCTB-12CupGrid-G2FarRight-G2Far-NA-0-NA</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-PCTB-4CupGridClose-G2FarLeft-NA-0-NA</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
     <t>OP-STC-Allo-PCTB-3CupFC-1G2LClose-DarkBlue-0-OpLava</t>
   </si>
   <si>
-    <t>OP-STC-Allo-PCTB-12CupGrid-G2FarLeft-G2Far-NA-0-NA</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-PCTB-4CupGridClose-G2FarRight-NA-0-NA</t>
   </si>
   <si>
@@ -543,6 +537,12 @@
   </si>
   <si>
     <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_2</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-12CupGrid-G2FarRightFar-NA-0-NA</t>
+  </si>
+  <si>
+    <t>OP-STC-Allo-PCTB-12CupGrid-G2FarLeftFar-NA-0-NA</t>
   </si>
 </sst>
 </file>
@@ -868,16 +868,19 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -895,19 +898,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1228,8 +1228,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AQ4" sqref="AQ4"/>
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,210 +1280,210 @@
   <sheetData>
     <row r="1" spans="1:98" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
-      <c r="C1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="X1" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="38"/>
-      <c r="AS1" s="38"/>
-      <c r="AT1" s="38"/>
-      <c r="AV1" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33"/>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33"/>
-      <c r="BA1" s="33"/>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="33"/>
-      <c r="BG1" s="33"/>
-      <c r="BH1" s="33"/>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33"/>
-      <c r="BL1" s="33"/>
-      <c r="BM1" s="33"/>
-      <c r="BN1" s="33"/>
-      <c r="BO1" s="33"/>
-      <c r="BP1" s="33"/>
-      <c r="BQ1" s="33"/>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="33"/>
-      <c r="BV1" s="33"/>
-      <c r="BW1" s="33"/>
-      <c r="BX1" s="33"/>
-      <c r="BY1" s="33"/>
-      <c r="BZ1" s="33"/>
-      <c r="CA1" s="33"/>
-      <c r="CB1" s="33"/>
-      <c r="CC1" s="33"/>
-      <c r="CD1" s="33"/>
-      <c r="CE1" s="33"/>
-      <c r="CF1" s="33"/>
-      <c r="CG1" s="33"/>
-      <c r="CH1" s="33"/>
-      <c r="CI1" s="33"/>
-      <c r="CJ1" s="33"/>
+      <c r="C1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="X1" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AV1" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW1" s="34"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="34"/>
+      <c r="AZ1" s="34"/>
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="34"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="34"/>
+      <c r="BT1" s="34"/>
+      <c r="BU1" s="34"/>
+      <c r="BV1" s="34"/>
+      <c r="BW1" s="34"/>
+      <c r="BX1" s="34"/>
+      <c r="BY1" s="34"/>
+      <c r="BZ1" s="34"/>
+      <c r="CA1" s="34"/>
+      <c r="CB1" s="34"/>
+      <c r="CC1" s="34"/>
+      <c r="CD1" s="34"/>
+      <c r="CE1" s="34"/>
+      <c r="CF1" s="34"/>
+      <c r="CG1" s="34"/>
+      <c r="CH1" s="34"/>
+      <c r="CI1" s="34"/>
+      <c r="CJ1" s="34"/>
     </row>
     <row r="2" spans="1:98" s="17" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="22" t="s">
+      <c r="Y2" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA2" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="Y2" s="23" t="s">
+      <c r="AB2" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC2" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE2" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF2" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH2" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI2" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ2" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK2" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="AL2" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM2" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AN2" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="AB2" s="23" t="s">
+      <c r="AO2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="AC2" s="23" t="s">
+      <c r="AP2" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="AD2" s="23" t="s">
+      <c r="AQ2" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="AE2" s="23" t="s">
+      <c r="AR2" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="AF2" s="23" t="s">
+      <c r="AS2" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="AG2" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="AH2" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI2" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ2" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK2" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL2" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="AM2" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN2" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="AO2" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="AP2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="AQ2" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="AR2" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="AS2" s="23" t="s">
-        <v>137</v>
-      </c>
       <c r="AT2" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="AU2" s="41" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="AU2" s="32" t="s">
+        <v>122</v>
       </c>
       <c r="AV2" s="16" t="s">
         <v>9</v>
@@ -1515,7 +1515,7 @@
       <c r="BE2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="BF2" s="39" t="s">
+      <c r="BF2" s="30" t="s">
         <v>19</v>
       </c>
       <c r="BG2" s="16" t="s">
@@ -1548,7 +1548,7 @@
       <c r="BP2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="BQ2" s="39" t="s">
+      <c r="BQ2" s="30" t="s">
         <v>30</v>
       </c>
       <c r="BR2" s="16" t="s">
@@ -1581,7 +1581,7 @@
       <c r="CA2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="CB2" s="39" t="s">
+      <c r="CB2" s="30" t="s">
         <v>41</v>
       </c>
       <c r="CC2" s="16" t="s">
@@ -1608,17 +1608,17 @@
       <c r="CJ2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="CK2" s="39" t="s">
-        <v>125</v>
+      <c r="CK2" s="30" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:98" s="11" customFormat="1" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="19" t="s">
         <v>84</v>
       </c>
@@ -1667,77 +1667,77 @@
       <c r="V3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="W3" s="32"/>
+      <c r="W3" s="42"/>
       <c r="X3" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y3" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC3" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="Y3" s="26" t="s">
+      <c r="AD3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="Z3" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AE3" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF3" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG3" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH3" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI3" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="AJ3" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK3" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="AB3" s="26" t="s">
+      <c r="AL3" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="AC3" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD3" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="AE3" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF3" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG3" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH3" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="AI3" s="26" t="s">
+      <c r="AM3" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="AJ3" s="26" t="s">
+      <c r="AO3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="AK3" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL3" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="AM3" s="26" t="s">
+      <c r="AP3" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="AN3" s="26" t="s">
+      <c r="AQ3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="AO3" s="26" t="s">
+      <c r="AR3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="AP3" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ3" s="26" t="s">
+      <c r="AS3" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="AR3" s="26" t="s">
+      <c r="AT3" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="AS3" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="AT3" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="AU3" s="42"/>
+      <c r="AU3" s="33"/>
       <c r="AV3" s="20" t="s">
         <v>101</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="AX3" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AY3" s="20" t="s">
         <v>103</v>
@@ -1760,63 +1760,63 @@
         <v>106</v>
       </c>
       <c r="BC3" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="BD3" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="BD3" s="20" t="s">
+      <c r="BE3" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="BF3" s="31"/>
+      <c r="BG3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="BE3" s="20" t="s">
+      <c r="BH3" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="BI3" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="BJ3" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="BK3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="BL3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="BM3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="BN3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="BO3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="BP3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="BQ3" s="31"/>
+      <c r="BR3" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="BT3" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="BF3" s="40"/>
-      <c r="BG3" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="BH3" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="BI3" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="BJ3" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="BK3" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="BL3" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="BM3" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="BN3" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="BO3" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="BP3" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="BQ3" s="40"/>
-      <c r="BR3" s="20" t="s">
+      <c r="BU3" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="BS3" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="BT3" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="BU3" s="20" t="s">
-        <v>119</v>
       </c>
       <c r="BV3" s="20" t="s">
         <v>102</v>
       </c>
       <c r="BW3" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="BX3" s="20" t="s">
         <v>104</v>
@@ -1825,37 +1825,37 @@
         <v>105</v>
       </c>
       <c r="BZ3" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="CA3" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="CB3" s="40"/>
+        <v>114</v>
+      </c>
+      <c r="CB3" s="31"/>
       <c r="CC3" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="CD3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="CE3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="CF3" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="CD3" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="CE3" s="20" t="s">
+      <c r="CG3" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="CF3" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="CG3" s="20" t="s">
-        <v>123</v>
-      </c>
       <c r="CH3" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="CI3" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="CJ3" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="CK3" s="40"/>
+        <v>108</v>
+      </c>
+      <c r="CK3" s="31"/>
       <c r="CL3" s="21"/>
       <c r="CM3" s="21"/>
       <c r="CN3" s="21"/>
@@ -9200,6 +9200,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="C1:V1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="X1:AT1"/>
     <mergeCell ref="CK2:CK3"/>
     <mergeCell ref="AU2:AU3"/>
@@ -9207,16 +9217,6 @@
     <mergeCell ref="BQ2:BQ3"/>
     <mergeCell ref="BF2:BF3"/>
     <mergeCell ref="AV1:CJ1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="O2:V2"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="C1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9224,25 +9224,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E74F6B21681AB408F9BC07DC9A0E55C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4c5f0e15b723777ad6492fe9c8c4393">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="03af05c1-6d5e-40c6-b524-3923c3d31a7d" xmlns:ns3="92fb2da0-1efd-490d-9574-64ca626f7778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffba0b7775c6a986b1b6d9a6ba35c06b" ns2:_="" ns3:_="">
     <xsd:import namespace="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
@@ -9447,25 +9428,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF44038-910F-4BF1-8B0A-E9EFAB10C83E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9482,4 +9464,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix minor error with task names for tutorial 7
</commit_message>
<xml_diff>
--- a/children/results_children.xlsx
+++ b/children/results_children.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kv301\Documents\comparative-object-permanence\children\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC728A0-371B-41F3-BA3A-67112864A102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B730F029-C7A4-4A11-A282-0A2DDFC476E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F7936E4C-9642-4CE6-A57D-FAC6EA268BDD}"/>
   </bookViews>
@@ -533,16 +533,16 @@
     <t>tutorial_4_3choicecylinder-G1.5-right_2</t>
   </si>
   <si>
-    <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_1</t>
-  </si>
-  <si>
-    <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_2</t>
-  </si>
-  <si>
     <t>OP-STC-Allo-PCTB-12CupGrid-G2FarRightFar-NA-0-NA</t>
   </si>
   <si>
     <t>OP-STC-Allo-PCTB-12CupGrid-G2FarLeftFar-NA-0-NA</t>
+  </si>
+  <si>
+    <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_variant_1</t>
+  </si>
+  <si>
+    <t>tutorial_7_OP-RP-Allo-CVChick-LOG31XtraLowIpsi-Right-RND-0-OPQ_variant_2</t>
   </si>
 </sst>
 </file>
@@ -868,19 +868,16 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -898,16 +895,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1228,8 +1228,8 @@
   <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH3" sqref="AH3"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,137 +1280,137 @@
   <sheetData>
     <row r="1" spans="1:98" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
-      <c r="C1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="X1" s="29" t="s">
+      <c r="C1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="X1" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AV1" s="34" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AV1" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34"/>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34"/>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="34"/>
-      <c r="BH1" s="34"/>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="34"/>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34"/>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="34"/>
-      <c r="BO1" s="34"/>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="34"/>
-      <c r="BT1" s="34"/>
-      <c r="BU1" s="34"/>
-      <c r="BV1" s="34"/>
-      <c r="BW1" s="34"/>
-      <c r="BX1" s="34"/>
-      <c r="BY1" s="34"/>
-      <c r="BZ1" s="34"/>
-      <c r="CA1" s="34"/>
-      <c r="CB1" s="34"/>
-      <c r="CC1" s="34"/>
-      <c r="CD1" s="34"/>
-      <c r="CE1" s="34"/>
-      <c r="CF1" s="34"/>
-      <c r="CG1" s="34"/>
-      <c r="CH1" s="34"/>
-      <c r="CI1" s="34"/>
-      <c r="CJ1" s="34"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="33"/>
+      <c r="BD1" s="33"/>
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="33"/>
+      <c r="BG1" s="33"/>
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="33"/>
+      <c r="BJ1" s="33"/>
+      <c r="BK1" s="33"/>
+      <c r="BL1" s="33"/>
+      <c r="BM1" s="33"/>
+      <c r="BN1" s="33"/>
+      <c r="BO1" s="33"/>
+      <c r="BP1" s="33"/>
+      <c r="BQ1" s="33"/>
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="33"/>
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="33"/>
+      <c r="BW1" s="33"/>
+      <c r="BX1" s="33"/>
+      <c r="BY1" s="33"/>
+      <c r="BZ1" s="33"/>
+      <c r="CA1" s="33"/>
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="33"/>
+      <c r="CD1" s="33"/>
+      <c r="CE1" s="33"/>
+      <c r="CF1" s="33"/>
+      <c r="CG1" s="33"/>
+      <c r="CH1" s="33"/>
+      <c r="CI1" s="33"/>
+      <c r="CJ1" s="33"/>
     </row>
     <row r="2" spans="1:98" s="17" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="41" t="s">
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="31" t="s">
         <v>8</v>
       </c>
       <c r="X2" s="22" t="s">
@@ -1482,7 +1482,7 @@
       <c r="AT2" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="AU2" s="32" t="s">
+      <c r="AU2" s="41" t="s">
         <v>122</v>
       </c>
       <c r="AV2" s="16" t="s">
@@ -1515,7 +1515,7 @@
       <c r="BE2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="BF2" s="30" t="s">
+      <c r="BF2" s="39" t="s">
         <v>19</v>
       </c>
       <c r="BG2" s="16" t="s">
@@ -1548,7 +1548,7 @@
       <c r="BP2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="BQ2" s="30" t="s">
+      <c r="BQ2" s="39" t="s">
         <v>30</v>
       </c>
       <c r="BR2" s="16" t="s">
@@ -1581,7 +1581,7 @@
       <c r="CA2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="CB2" s="30" t="s">
+      <c r="CB2" s="39" t="s">
         <v>41</v>
       </c>
       <c r="CC2" s="16" t="s">
@@ -1608,17 +1608,17 @@
       <c r="CJ2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="CK2" s="30" t="s">
+      <c r="CK2" s="39" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:98" s="11" customFormat="1" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="19" t="s">
         <v>84</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="V3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="W3" s="42"/>
+      <c r="W3" s="32"/>
       <c r="X3" s="25" t="s">
         <v>139</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>142</v>
       </c>
       <c r="AE3" s="26" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AF3" s="26" t="s">
         <v>143</v>
@@ -1723,7 +1723,7 @@
         <v>149</v>
       </c>
       <c r="AP3" s="26" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AQ3" s="26" t="s">
         <v>150</v>
@@ -1737,7 +1737,7 @@
       <c r="AT3" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="AU3" s="33"/>
+      <c r="AU3" s="42"/>
       <c r="AV3" s="20" t="s">
         <v>101</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>106</v>
       </c>
       <c r="BC3" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BD3" s="20" t="s">
         <v>107</v>
@@ -1768,7 +1768,7 @@
       <c r="BE3" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="BF3" s="31"/>
+      <c r="BF3" s="40"/>
       <c r="BG3" s="20" t="s">
         <v>108</v>
       </c>
@@ -1799,7 +1799,7 @@
       <c r="BP3" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="BQ3" s="31"/>
+      <c r="BQ3" s="40"/>
       <c r="BR3" s="20" t="s">
         <v>117</v>
       </c>
@@ -1830,9 +1830,9 @@
       <c r="CA3" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="CB3" s="31"/>
+      <c r="CB3" s="40"/>
       <c r="CC3" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="CD3" s="20" t="s">
         <v>112</v>
@@ -1855,7 +1855,7 @@
       <c r="CJ3" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="CK3" s="31"/>
+      <c r="CK3" s="40"/>
       <c r="CL3" s="21"/>
       <c r="CM3" s="21"/>
       <c r="CN3" s="21"/>
@@ -9200,16 +9200,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="O2:V2"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="C1:V1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="X1:AT1"/>
     <mergeCell ref="CK2:CK3"/>
     <mergeCell ref="AU2:AU3"/>
@@ -9217,6 +9207,16 @@
     <mergeCell ref="BQ2:BQ3"/>
     <mergeCell ref="BF2:BF3"/>
     <mergeCell ref="AV1:CJ1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="C1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9224,6 +9224,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E74F6B21681AB408F9BC07DC9A0E55C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4c5f0e15b723777ad6492fe9c8c4393">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="03af05c1-6d5e-40c6-b524-3923c3d31a7d" xmlns:ns3="92fb2da0-1efd-490d-9574-64ca626f7778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffba0b7775c6a986b1b6d9a6ba35c06b" ns2:_="" ns3:_="">
     <xsd:import namespace="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
@@ -9428,26 +9447,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03af05c1-6d5e-40c6-b524-3923c3d31a7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF44038-910F-4BF1-8B0A-E9EFAB10C83E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9464,22 +9482,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6D725A-C8B9-4A8E-B1D4-AB4EC439C715}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="03af05c1-6d5e-40c6-b524-3923c3d31a7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17E392F8-A54D-4C0D-B0FB-83806B26E3F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>